<commit_message>
added more entities for WGs; added ref entities
</commit_message>
<xml_diff>
--- a/dist/rd3_cluster.xlsx
+++ b/dist/rd3_cluster.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
   <si>
     <t>rd3_cluster</t>
   </si>
@@ -36,24 +36,117 @@
     <t>Metadata on files produced by working group(v1.0.0, 2022-09-15)</t>
   </si>
   <si>
+    <t>erns</t>
+  </si>
+  <si>
+    <t>filetypes</t>
+  </si>
+  <si>
     <t>template</t>
   </si>
   <si>
+    <t>cnv</t>
+  </si>
+  <si>
+    <t>denovo</t>
+  </si>
+  <si>
+    <t>proteomics</t>
+  </si>
+  <si>
+    <t>roh</t>
+  </si>
+  <si>
     <t>snvindel</t>
   </si>
   <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>transcriptomics</t>
+  </si>
+  <si>
+    <t>ERNS</t>
+  </si>
+  <si>
+    <t>File Types</t>
+  </si>
+  <si>
+    <t>CNV</t>
+  </si>
+  <si>
+    <t>Denovo</t>
+  </si>
+  <si>
+    <t>Proteomics</t>
+  </si>
+  <si>
+    <t>ROH Relatedness</t>
+  </si>
+  <si>
+    <t>SNV-Indel</t>
+  </si>
+  <si>
+    <t>STR</t>
+  </si>
+  <si>
+    <t>Transcriptomics</t>
+  </si>
+  <si>
+    <t>Reference table for European Reference Networks</t>
+  </si>
+  <si>
+    <t>Reference table for known file types</t>
+  </si>
+  <si>
     <t>attribute template for listing files by working group</t>
   </si>
   <si>
-    <t>Files produced by the SNV-Indel working group</t>
-  </si>
-  <si>
-    <t>SNV-Indel</t>
+    <t>CNV working group files</t>
+  </si>
+  <si>
+    <t>Denovo working group file</t>
+  </si>
+  <si>
+    <t>Proteomics working group files</t>
+  </si>
+  <si>
+    <t>ROG Relatedness working group files</t>
+  </si>
+  <si>
+    <t>SNV-Indel working group files</t>
+  </si>
+  <si>
+    <t>STR working group files</t>
+  </si>
+  <si>
+    <t>Transcriptomics working group files</t>
   </si>
   <si>
     <t>rd3_cluster_results_template</t>
   </si>
   <si>
+    <t>rd3_cluster_erns</t>
+  </si>
+  <si>
+    <t>rd3_cluster_filetypes</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>shortname</t>
+  </si>
+  <si>
+    <t>fullname</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
     <t>inode</t>
   </si>
   <si>
@@ -75,6 +168,15 @@
     <t>size</t>
   </si>
   <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>xref</t>
+  </si>
+  <si>
     <t>unique identifier of a file in a specific location</t>
   </si>
   <si>
@@ -93,18 +195,15 @@
     <t>file extension</t>
   </si>
   <si>
-    <t>size of the file (in bytes)</t>
-  </si>
-  <si>
-    <t>string</t>
+    <t>size of the file (in kilobytes)</t>
+  </si>
+  <si>
+    <t>size (kb)</t>
   </si>
   <si>
     <t>label</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>parent</t>
   </si>
   <si>
@@ -120,13 +219,25 @@
     <t>entity</t>
   </si>
   <si>
+    <t>idAttribute</t>
+  </si>
+  <si>
     <t>dataType</t>
   </si>
   <si>
-    <t>idAttribute</t>
-  </si>
-  <si>
     <t>labelAttribute</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>lookupAttribute</t>
+  </si>
+  <si>
+    <t>refEntity</t>
   </si>
 </sst>
 </file>
@@ -481,16 +592,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -525,7 +636,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -533,53 +644,183 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="b">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -589,81 +830,108 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
       <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
+        <v>38</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="E2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
+        <v>39</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="E3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
+        <v>40</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -671,33 +939,48 @@
       <c r="F4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
+        <v>41</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
       </c>
       <c r="E5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
+        <v>42</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -705,39 +988,148 @@
       <c r="F6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
+        <v>43</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
       </c>
-      <c r="F7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="I7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
+        <v>44</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
       </c>
-      <c r="F8" t="b">
-        <v>0</v>
+      <c r="I8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed data type to text
</commit_message>
<xml_diff>
--- a/dist/rd3_cluster.xlsx
+++ b/dist/rd3_cluster.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="74">
   <si>
     <t>rd3_cluster</t>
   </si>
@@ -33,7 +33,7 @@
     <t>Information and data on the contents of the cluster (Fender)(v1.0.0, 2022-09-15)</t>
   </si>
   <si>
-    <t>Metadata on files produced by working group(v1.0.0, 2022-09-15)</t>
+    <t>Metadata on files produced by working group(v1.1.0, 2022-09-19)</t>
   </si>
   <si>
     <t>erns</t>
@@ -1082,6 +1082,9 @@
       <c r="C11" t="b">
         <v>0</v>
       </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
       <c r="E11" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
added new entities; changed xref to categorical
</commit_message>
<xml_diff>
--- a/dist/rd3_cluster.xlsx
+++ b/dist/rd3_cluster.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="80">
   <si>
     <t>rd3_cluster</t>
   </si>
@@ -33,7 +33,7 @@
     <t>Information and data on the contents of the cluster (Fender)(v1.0.0, 2022-09-15)</t>
   </si>
   <si>
-    <t>Metadata on files produced by working group(v1.1.0, 2022-09-19)</t>
+    <t>Metadata on files produced by working group(v1.2.0, 2022-09-20)</t>
   </si>
   <si>
     <t>erns</t>
@@ -51,12 +51,18 @@
     <t>denovo</t>
   </si>
   <si>
+    <t>meta</t>
+  </si>
+  <si>
     <t>proteomics</t>
   </si>
   <si>
     <t>roh</t>
   </si>
   <si>
+    <t>sandbox</t>
+  </si>
+  <si>
     <t>snvindel</t>
   </si>
   <si>
@@ -78,12 +84,18 @@
     <t>Denovo</t>
   </si>
   <si>
+    <t>Meta Analysis</t>
+  </si>
+  <si>
     <t>Proteomics</t>
   </si>
   <si>
     <t>ROH Relatedness</t>
   </si>
   <si>
+    <t>Sandbox</t>
+  </si>
+  <si>
     <t>SNV-Indel</t>
   </si>
   <si>
@@ -105,7 +117,10 @@
     <t>CNV working group files</t>
   </si>
   <si>
-    <t>Denovo working group file</t>
+    <t>Denovo working group files</t>
+  </si>
+  <si>
+    <t>Meta Analysis working group files</t>
   </si>
   <si>
     <t>Proteomics working group files</t>
@@ -114,6 +129,9 @@
     <t>ROG Relatedness working group files</t>
   </si>
   <si>
+    <t>Sandbox only files</t>
+  </si>
+  <si>
     <t>SNV-Indel working group files</t>
   </si>
   <si>
@@ -174,7 +192,7 @@
     <t>text</t>
   </si>
   <si>
-    <t>xref</t>
+    <t>categorical</t>
   </si>
   <si>
     <t>unique identifier of a file in a specific location</t>
@@ -592,16 +610,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -636,7 +654,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -644,22 +662,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -670,10 +688,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -684,10 +702,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -698,7 +716,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -712,13 +730,13 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -729,13 +747,13 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -746,13 +764,13 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -763,13 +781,13 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -780,13 +798,13 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -797,13 +815,13 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -814,13 +832,47 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -838,51 +890,51 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -896,16 +948,16 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -922,16 +974,16 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -945,16 +997,16 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -971,16 +1023,16 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -994,73 +1046,73 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="J9" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -1069,58 +1121,58 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="J12" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -1129,10 +1181,10 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="K13" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>